<commit_message>
adding options risk new
</commit_message>
<xml_diff>
--- a/FromPython.xlsx
+++ b/FromPython.xlsx
@@ -1,43 +1,66 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14900" tabRatio="500"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="From Python" sheetId="1" r:id="rId1"/>
+    <sheet name="From Python" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>PnL</t>
+  </si>
+  <si>
+    <t>Perf</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
+    <numFmt formatCode="YYYY-MM-DD HH:MM:SS" numFmtId="165"/>
+  </numFmts>
+  <fonts count="2">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,18 +68,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="3">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -135,7 +170,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -170,7 +204,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -205,16 +238,20 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -336,63 +373,430 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2" t="n">
+        <v>43487.77083333334</v>
+      </c>
+      <c r="B2" t="n">
+        <v>11.04</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s"/>
+      <c r="E2" t="s"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2" t="n">
+        <v>43487.8125</v>
+      </c>
+      <c r="B3" t="n">
+        <v>11.14</v>
+      </c>
+      <c r="C3" t="n">
+        <v>-62117</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-6211.700000000088</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-6211.700000000088</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2" t="n">
+        <v>43487.85416666666</v>
+      </c>
+      <c r="B4" t="n">
+        <v>11.11</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-6211.700000000088</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="2" t="n">
+        <v>43487.89583333334</v>
+      </c>
+      <c r="B5" t="n">
+        <v>11.11</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-6211.700000000088</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2" t="n">
+        <v>43487.9375</v>
+      </c>
+      <c r="B6" t="n">
+        <v>11.11</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-6211.700000000088</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2" t="n">
+        <v>43487.97916666666</v>
+      </c>
+      <c r="B7" t="n">
+        <v>11.11</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-6211.700000000088</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2" t="n">
+        <v>43488.02083333334</v>
+      </c>
+      <c r="B8" t="n">
+        <v>11.11</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-6211.700000000088</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2" t="n">
+        <v>43488.0625</v>
+      </c>
+      <c r="B9" t="n">
+        <v>11.11</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-6211.700000000088</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="2" t="n">
+        <v>43488.10416666666</v>
+      </c>
+      <c r="B10" t="n">
+        <v>11.11</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-6211.700000000088</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="2" t="n">
+        <v>43488.14583333334</v>
+      </c>
+      <c r="B11" t="n">
+        <v>11.11</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-6211.700000000088</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="2" t="n">
+        <v>43488.1875</v>
+      </c>
+      <c r="B12" t="n">
+        <v>11.11</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-6211.700000000088</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="2" t="n">
+        <v>43488.22916666666</v>
+      </c>
+      <c r="B13" t="n">
+        <v>11.11</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-6211.700000000088</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="2" t="n">
+        <v>43488.27083333334</v>
+      </c>
+      <c r="B14" t="n">
+        <v>11.11</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-6211.700000000088</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="2" t="n">
+        <v>43488.3125</v>
+      </c>
+      <c r="B15" t="n">
+        <v>11.11</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-6211.700000000088</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="2" t="n">
+        <v>43488.35416666666</v>
+      </c>
+      <c r="B16" t="n">
+        <v>11.11</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-6211.700000000088</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="2" t="n">
+        <v>43488.39583333334</v>
+      </c>
+      <c r="B17" t="n">
+        <v>11.11</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-6211.700000000088</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="2" t="n">
+        <v>43488.4375</v>
+      </c>
+      <c r="B18" t="n">
+        <v>11.11</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-6211.700000000088</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="2" t="n">
+        <v>43488.47916666666</v>
+      </c>
+      <c r="B19" t="n">
+        <v>11.11</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>-6211.700000000088</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="2" t="n">
+        <v>43488.52083333334</v>
+      </c>
+      <c r="B20" t="n">
+        <v>11.11</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>-6211.700000000088</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="2" t="n">
+        <v>43488.5625</v>
+      </c>
+      <c r="B21" t="n">
+        <v>11.11</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>-6211.700000000088</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="2" t="n">
+        <v>43488.60416666666</v>
+      </c>
+      <c r="B22" t="n">
+        <v>11.18</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>-6211.700000000088</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="2" t="n">
+        <v>43488.64583333334</v>
+      </c>
+      <c r="B23" t="n">
+        <v>11.11</v>
+      </c>
+      <c r="C23" t="n">
+        <v>-64068</v>
+      </c>
+      <c r="D23" t="n">
+        <v>4484.760000000018</v>
+      </c>
+      <c r="E23" t="n">
+        <v>-1726.94000000007</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="2" t="n">
+        <v>43488.6875</v>
+      </c>
+      <c r="B24" t="n">
+        <v>11.03</v>
+      </c>
+      <c r="C24" t="n">
+        <v>59904</v>
+      </c>
+      <c r="D24" t="n">
+        <v>-4792.320000000004</v>
+      </c>
+      <c r="E24" t="n">
+        <v>-6519.260000000074</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>